<commit_message>
Add new example data BEXSTATEST2
</commit_message>
<xml_diff>
--- a/data-raw/metadata/metadata_BEXSTATEST2.xlsx
+++ b/data-raw/metadata/metadata_BEXSTATEST2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/672a29ec829a16e8/Dokumenter/GitHub/ProjCore/px/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\px\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{957DD5BA-BFB5-45AF-A480-BE77E2B322D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E99D7944-53ED-4655-8D0C-B0EEE390B78D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BE8216-F81B-462C-BDF9-D81B6B61AB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17265" yWindow="1080" windowWidth="23220" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -929,7 +929,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Link 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -946,12 +946,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1273,13 +1269,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1328125"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
@@ -1606,9 +1601,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -4108,11 +4105,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -4406,7 +4403,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>

</xml_diff>

<commit_message>
Remove unused variables from codelist in metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/metadata_BEXSTATEST2.xlsx
+++ b/data-raw/metadata/metadata_BEXSTATEST2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\px\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BE8216-F81B-462C-BDF9-D81B6B61AB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD039892-EA16-4891-A771-3B7D9E4407A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17265" yWindow="1080" windowWidth="23220" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="31800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="264">
   <si>
     <t>VarName</t>
   </si>
@@ -79,9 +79,6 @@
     <t>antal</t>
   </si>
   <si>
-    <t>bosted</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -574,39 +571,12 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Town</t>
-  </si>
-  <si>
-    <t>Settlement</t>
-  </si>
-  <si>
-    <t>Station</t>
-  </si>
-  <si>
-    <t>Farm</t>
-  </si>
-  <si>
     <t>I alt</t>
   </si>
   <si>
-    <t>By</t>
-  </si>
-  <si>
-    <t>Bygd</t>
-  </si>
-  <si>
-    <t>Fårehold</t>
-  </si>
-  <si>
     <t>Katillugit</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>Uoplyst</t>
-  </si>
-  <si>
     <t>Greenland</t>
   </si>
   <si>
@@ -664,21 +634,6 @@
     <t>VPUkiut</t>
   </si>
   <si>
-    <t>Illoqarfik</t>
-  </si>
-  <si>
-    <t>Nunaqarfik</t>
-  </si>
-  <si>
-    <t>Paasissutissaqanngitsut</t>
-  </si>
-  <si>
-    <t>Savaateqarfik</t>
-  </si>
-  <si>
-    <t>Stationi</t>
-  </si>
-  <si>
     <t>1. Januaarimi innuttaasut</t>
   </si>
   <si>
@@ -752,15 +707,6 @@
   </si>
   <si>
     <t>Other localities</t>
-  </si>
-  <si>
-    <t>BSTED</t>
-  </si>
-  <si>
-    <t>Øvrige</t>
-  </si>
-  <si>
-    <t>Other</t>
   </si>
   <si>
     <t>bostedstype</t>
@@ -1269,7 +1215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -1283,7 +1229,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1330,19 +1276,19 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
@@ -1357,27 +1303,27 @@
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="K2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="L2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="O2" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -1386,10 +1332,10 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G3" t="s">
         <v>15</v>
@@ -1421,31 +1367,31 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="B4" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="C4" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="D4" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="E4" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="F4" t="s">
         <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L4" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="M4" t="s">
         <v>15</v>
@@ -1459,19 +1405,19 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F5" t="s">
         <v>16</v>
@@ -1486,13 +1432,13 @@
         <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L5" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="M5" t="s">
         <v>15</v>
@@ -1506,19 +1452,19 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="B6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -1533,13 +1479,13 @@
         <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L6" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="M6" t="s">
         <v>15</v>
@@ -1553,22 +1499,22 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G7" t="s">
         <v>15</v>
@@ -1599,10 +1545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1618,2482 +1564,2302 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
       <c r="G1" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B16">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B23">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B24">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B26">
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B28">
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B29">
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B30">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B31">
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B32">
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B33">
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B34">
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B35">
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B36">
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B37">
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B38">
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B39">
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B40">
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B41">
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B42">
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B43">
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B44">
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B45">
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B46">
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B47">
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B48">
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B49">
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B50">
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B51">
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B52">
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B53">
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B54">
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B55">
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B56">
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B57">
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B58">
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B59">
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B60">
         <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B61">
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B62">
         <v>60</v>
       </c>
       <c r="C62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B63">
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F63" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B64">
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B65">
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B66">
         <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B67">
         <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B68">
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B69">
         <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B70">
         <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B71">
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B72">
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F72" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B73">
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F73" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B74">
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F74" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B75">
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B76">
         <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B77">
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B78">
         <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F78" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B79">
         <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F79" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B80">
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F80" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B81">
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B82">
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B83">
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F83" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B84">
         <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B85">
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B86">
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B87">
         <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D87" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E87" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F87" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B88">
         <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B89">
         <v>87</v>
       </c>
       <c r="C89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B90">
         <v>88</v>
       </c>
       <c r="C90" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D90" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E90" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F90" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B91">
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F91" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B92">
         <v>90</v>
       </c>
       <c r="C92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F92" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B93">
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B94">
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B95">
         <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F95" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B96">
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D96" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E96" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F96" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B97">
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D97" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E97" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F97" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B98">
         <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D98" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E98" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F98" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B99">
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D99" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E99" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F99" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B100">
         <v>98</v>
       </c>
       <c r="C100" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D100" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E100" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F100" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B101">
         <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D101" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E101" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F101" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>18</v>
+        <v>172</v>
       </c>
       <c r="B102">
         <v>0</v>
       </c>
       <c r="C102" t="s">
-        <v>24</v>
+        <v>204</v>
       </c>
       <c r="D102" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E102" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F102" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>18</v>
+        <v>172</v>
       </c>
       <c r="B103">
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>25</v>
+        <v>123</v>
       </c>
       <c r="D103" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E103" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F103" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>18</v>
+        <v>172</v>
       </c>
       <c r="B104">
         <v>2</v>
       </c>
       <c r="C104" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="D104" t="s">
+        <v>188</v>
+      </c>
+      <c r="E104" t="s">
+        <v>187</v>
+      </c>
+      <c r="F104" t="s">
         <v>189</v>
-      </c>
-      <c r="E104" t="s">
-        <v>184</v>
-      </c>
-      <c r="F104" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>18</v>
+        <v>171</v>
       </c>
       <c r="B105">
-        <v>3</v>
-      </c>
-      <c r="C105" t="s">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="D105" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E105" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F105" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>18</v>
+        <v>171</v>
       </c>
       <c r="B106">
-        <v>4</v>
-      </c>
-      <c r="C106" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>205</v>
       </c>
       <c r="D106" t="s">
+        <v>192</v>
+      </c>
+      <c r="E106" t="s">
         <v>190</v>
       </c>
-      <c r="E106" t="s">
-        <v>186</v>
-      </c>
       <c r="F106" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>18</v>
+        <v>171</v>
       </c>
       <c r="B107">
-        <v>5</v>
-      </c>
-      <c r="C107" t="s">
-        <v>33</v>
+        <v>2</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="D107" t="s">
         <v>193</v>
       </c>
       <c r="E107" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F107" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>173</v>
+        <v>263</v>
       </c>
       <c r="B108">
         <v>0</v>
       </c>
       <c r="C108" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="D108" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E108" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F108" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>173</v>
+        <v>263</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>124</v>
+        <v>229</v>
       </c>
       <c r="D109" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="E109" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="F109" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>173</v>
+        <v>263</v>
       </c>
       <c r="B110">
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>125</v>
+        <v>230</v>
       </c>
       <c r="D110" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
       <c r="E110" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="F110" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>263</v>
       </c>
       <c r="B111">
-        <v>0</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>219</v>
+        <v>3</v>
+      </c>
+      <c r="C111" t="s">
+        <v>231</v>
       </c>
       <c r="D111" t="s">
-        <v>187</v>
+        <v>215</v>
       </c>
       <c r="E111" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="F111" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>263</v>
       </c>
       <c r="B112">
-        <v>1</v>
-      </c>
-      <c r="C112" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C112" t="s">
+        <v>232</v>
+      </c>
+      <c r="D112" t="s">
+        <v>218</v>
+      </c>
+      <c r="E112" t="s">
+        <v>219</v>
+      </c>
+      <c r="F112" t="s">
         <v>220</v>
-      </c>
-      <c r="D112" t="s">
-        <v>202</v>
-      </c>
-      <c r="E112" t="s">
-        <v>200</v>
-      </c>
-      <c r="F112" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>172</v>
+        <v>263</v>
       </c>
       <c r="B113">
-        <v>2</v>
-      </c>
-      <c r="C113" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" t="s">
+        <v>233</v>
+      </c>
+      <c r="D113" t="s">
         <v>221</v>
       </c>
-      <c r="D113" t="s">
-        <v>203</v>
-      </c>
       <c r="E113" t="s">
-        <v>201</v>
+        <v>222</v>
       </c>
       <c r="F113" t="s">
-        <v>205</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="D114" t="s">
-        <v>187</v>
+        <v>236</v>
       </c>
       <c r="E114" t="s">
-        <v>182</v>
+        <v>224</v>
       </c>
       <c r="F114" t="s">
-        <v>191</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="B115">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C115" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D115" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E115" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F115" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
-      <c r="A116" t="s">
-        <v>281</v>
-      </c>
-      <c r="B116">
-        <v>2</v>
-      </c>
-      <c r="C116" t="s">
-        <v>248</v>
-      </c>
-      <c r="D116" t="s">
-        <v>227</v>
-      </c>
-      <c r="E116" t="s">
-        <v>228</v>
-      </c>
-      <c r="F116" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
-      <c r="A117" t="s">
-        <v>281</v>
-      </c>
-      <c r="B117">
-        <v>3</v>
-      </c>
-      <c r="C117" t="s">
-        <v>249</v>
-      </c>
-      <c r="D117" t="s">
-        <v>230</v>
-      </c>
-      <c r="E117" t="s">
-        <v>231</v>
-      </c>
-      <c r="F117" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
-      <c r="A118" t="s">
-        <v>281</v>
-      </c>
-      <c r="B118">
-        <v>4</v>
-      </c>
-      <c r="C118" t="s">
-        <v>250</v>
-      </c>
-      <c r="D118" t="s">
-        <v>233</v>
-      </c>
-      <c r="E118" t="s">
-        <v>234</v>
-      </c>
-      <c r="F118" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
-      <c r="A119" t="s">
-        <v>281</v>
-      </c>
-      <c r="B119">
-        <v>5</v>
-      </c>
-      <c r="C119" t="s">
-        <v>251</v>
-      </c>
-      <c r="D119" t="s">
-        <v>236</v>
-      </c>
-      <c r="E119" t="s">
-        <v>237</v>
-      </c>
-      <c r="F119" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120" t="s">
-        <v>281</v>
-      </c>
-      <c r="B120">
-        <v>6</v>
-      </c>
-      <c r="C120" t="s">
-        <v>252</v>
-      </c>
-      <c r="D120" t="s">
-        <v>254</v>
-      </c>
-      <c r="E120" t="s">
-        <v>239</v>
-      </c>
-      <c r="F120" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" t="s">
-        <v>281</v>
-      </c>
-      <c r="B121">
-        <v>7</v>
-      </c>
-      <c r="C121" t="s">
-        <v>253</v>
-      </c>
-      <c r="D121" t="s">
-        <v>241</v>
-      </c>
-      <c r="E121" t="s">
-        <v>242</v>
-      </c>
-      <c r="F121" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" t="s">
-        <v>243</v>
-      </c>
-      <c r="B122">
-        <v>1</v>
-      </c>
-      <c r="C122" t="s">
-        <v>25</v>
-      </c>
-      <c r="D122" t="s">
-        <v>188</v>
-      </c>
-      <c r="E122" t="s">
-        <v>183</v>
-      </c>
-      <c r="F122" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" t="s">
-        <v>243</v>
-      </c>
-      <c r="B123">
-        <v>2</v>
-      </c>
-      <c r="C123" t="s">
-        <v>26</v>
-      </c>
-      <c r="D123" t="s">
-        <v>189</v>
-      </c>
-      <c r="E123" t="s">
-        <v>184</v>
-      </c>
-      <c r="F123" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" t="s">
-        <v>243</v>
-      </c>
-      <c r="B124">
-        <v>9</v>
-      </c>
-      <c r="C124" t="s">
-        <v>33</v>
-      </c>
-      <c r="D124" t="s">
-        <v>244</v>
-      </c>
-      <c r="E124" t="s">
-        <v>245</v>
-      </c>
-      <c r="F124" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4117,23 +3883,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" t="s">
         <v>126</v>
-      </c>
-      <c r="B1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="B2" t="s">
-        <v>269</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="B3" s="4">
         <v>2000</v>
@@ -4141,215 +3907,215 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>255</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="B6" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
         <v>137</v>
-      </c>
-      <c r="B16" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" t="s">
         <v>139</v>
-      </c>
-      <c r="B17" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" t="s">
         <v>141</v>
-      </c>
-      <c r="B18" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B24" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B25" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B27" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B29" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4357,7 +4123,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -4365,26 +4131,26 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -4416,16 +4182,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" t="s">
         <v>157</v>
-      </c>
-      <c r="E1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>